<commit_message>
Rev 1 design finished
</commit_message>
<xml_diff>
--- a/BOM/BOM UPZ Mouse.xlsx
+++ b/BOM/BOM UPZ Mouse.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\UPZ_Switcher\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\UPL_Mouse\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F88592-42CD-44F6-9B0A-C4F97A72F6D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C981CE-986B-434F-9AD5-B80439B2ECE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
   </bookViews>
   <sheets>
-    <sheet name="FetHead" sheetId="3" r:id="rId1"/>
+    <sheet name="UPL Mouse" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Description</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>RSComponents</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -63,106 +60,31 @@
     <t>Type</t>
   </si>
   <si>
-    <t>NC3FDH</t>
-  </si>
-  <si>
-    <t>XLR</t>
-  </si>
-  <si>
-    <t>NC3MDH</t>
-  </si>
-  <si>
-    <t>861-4281</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>LED Green Red</t>
-  </si>
-  <si>
-    <t>LED Yellow Red</t>
-  </si>
-  <si>
-    <t>861-4278</t>
-  </si>
-  <si>
-    <t>446-5243</t>
-  </si>
-  <si>
-    <t>DB9</t>
-  </si>
-  <si>
-    <t>TQ2SA-5V</t>
-  </si>
-  <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>DB9 connector</t>
-  </si>
-  <si>
-    <t>Mosfet</t>
-  </si>
-  <si>
-    <t>B170</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>6K8 Phantom</t>
-  </si>
-  <si>
-    <t>1K Mosfet</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>10nF Mosfet</t>
-  </si>
-  <si>
-    <t>MicroController</t>
-  </si>
-  <si>
-    <t>Arduino Micro</t>
-  </si>
-  <si>
-    <t>IO Expander</t>
-  </si>
-  <si>
-    <t>MCP23017</t>
-  </si>
-  <si>
-    <t>DIP Socket</t>
-  </si>
-  <si>
-    <t>28 Pin Small</t>
-  </si>
-  <si>
-    <t>29 Pin Wide</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>4K7</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>DIP Switch</t>
-  </si>
-  <si>
-    <t>Address selector</t>
+    <t>5749180-1</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>Mini Din 6</t>
+  </si>
+  <si>
+    <t>MAX232DR</t>
+  </si>
+  <si>
+    <t>attiny85</t>
+  </si>
+  <si>
+    <t>microUSB</t>
+  </si>
+  <si>
+    <t>capacitors 1uF</t>
+  </si>
+  <si>
+    <t>Header 3x2</t>
+  </si>
+  <si>
+    <t>DB9 Female</t>
   </si>
 </sst>
 </file>
@@ -213,9 +135,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,14 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B339EA2E-58E6-48C2-B743-24C662D28A88}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
@@ -548,10 +472,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -588,310 +512,157 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.68</v>
+      </c>
+      <c r="F3">
+        <f>D3*E3</f>
+        <v>1.68</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>4.92</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>39.36</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="A4" s="1">
+        <v>3121254</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>4.7699999999999996</v>
+        <v>0.86</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>9.5399999999999991</v>
+        <v>0.86</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1">
+        <v>1972176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.08</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2751675</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.27</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2357339</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="E5">
-        <v>0.128</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F6" si="1">D5*E5</f>
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="E7">
-        <v>2.3199999999999998</v>
+        <v>0.156</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
+        <v>0.624</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
+      <c r="A8" s="1">
+        <v>2751377</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <f>8+8+2</f>
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>3.17</v>
+        <v>1.86</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>57.06</v>
+        <v>1.86</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
       <c r="D9">
-        <f>D8</f>
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11">
-        <f>D9</f>
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <f>D11</f>
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20">
-        <v>18</v>
-      </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23">
-        <f>SUM(F2:F15)</f>
-        <v>108.93600000000001</v>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F2:F8)</f>
+        <v>6.3740000000000006</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{AD3496D0-3AB9-4E69-AC55-E94813676579}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{A02C7244-D8B9-40AB-8FC8-DEAFD07974B3}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{E2948649-F1C0-4F6A-B92B-78B6B61FB400}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{2200234E-19C1-4A6D-A257-A8DB47B48A2E}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{DBD43EE4-2E7F-42F4-ADDF-9E01CDD356B7}"/>
-    <hyperlink ref="A8" r:id="rId6" xr:uid="{7C032C1A-3DAB-485E-B8EB-E9C947593005}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{0B29A241-298C-4995-BA8C-F9A8987BD0A2}"/>
+    <hyperlink ref="A4" r:id="rId2" display="3121254" xr:uid="{DCE07E39-FF29-4113-8E14-7032851E32BE}"/>
+    <hyperlink ref="A6" r:id="rId3" display="2751675" xr:uid="{A123E1AB-3FCE-4EB9-833F-A07B40A3DA88}"/>
+    <hyperlink ref="A5" r:id="rId4" display="1972176" xr:uid="{36712850-C27E-41B7-95B4-5CAC5D8878D9}"/>
+    <hyperlink ref="A7" r:id="rId5" display="2357339" xr:uid="{52BCC742-C6E0-4A6A-A469-C0C23A30453C}"/>
+    <hyperlink ref="A8" r:id="rId6" display="2751377" xr:uid="{08B428DC-AE67-4862-A652-337615C869C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>